<commit_message>
small update of the user stories
</commit_message>
<xml_diff>
--- a/laravel_user_stories_v20191120.xlsx
+++ b/laravel_user_stories_v20191120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthijsberghuis/bap-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5686561E-45C3-DA42-82D5-461C892A2FB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F011C9F-C9C9-6F47-9105-0531C4892B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{96E4F204-A96B-B442-B776-0E7F469FE00D}"/>
   </bookViews>
@@ -1536,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F8C07C-95E6-5F45-AA16-00A7B9F9E844}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="94" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>188</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>31</v>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>188</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>32</v>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>188</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>33</v>

</xml_diff>